<commit_message>
ver 0.021 ažurani podaci iz google sheeta
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mihas\Programming\Python\Projects\KPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4B307F-8A69-4CF1-AF2A-27BA4EDA24ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05EEBF-6E83-43B0-807E-68235DD8F1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{5EDA8619-E0A5-4851-A543-B76F1F64E136}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EDA8619-E0A5-4851-A543-B76F1F64E136}"/>
   </bookViews>
   <sheets>
     <sheet name="pripremljen 2021 2022" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="661">
   <si>
     <t>Br.</t>
   </si>
@@ -1841,6 +1841,189 @@
   </si>
   <si>
     <t>c_user</t>
+  </si>
+  <si>
+    <t>30.08.2022.</t>
+  </si>
+  <si>
+    <t>22-0157</t>
+  </si>
+  <si>
+    <t>22-0158</t>
+  </si>
+  <si>
+    <t>22-0159</t>
+  </si>
+  <si>
+    <t>22-0160</t>
+  </si>
+  <si>
+    <t>22-0161</t>
+  </si>
+  <si>
+    <t>01.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0162</t>
+  </si>
+  <si>
+    <t>22-0163</t>
+  </si>
+  <si>
+    <t>22-0164</t>
+  </si>
+  <si>
+    <t>22-0165</t>
+  </si>
+  <si>
+    <t>22-0166</t>
+  </si>
+  <si>
+    <t>22-0167</t>
+  </si>
+  <si>
+    <t>22-0168</t>
+  </si>
+  <si>
+    <t>22-0169</t>
+  </si>
+  <si>
+    <t>22-0170</t>
+  </si>
+  <si>
+    <t>Ekonomsko-tehnička škola</t>
+  </si>
+  <si>
+    <t>22-0171</t>
+  </si>
+  <si>
+    <t>06.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0172</t>
+  </si>
+  <si>
+    <t>OŠ Jovan Cvijić</t>
+  </si>
+  <si>
+    <t>12.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0173</t>
+  </si>
+  <si>
+    <t>22-0174</t>
+  </si>
+  <si>
+    <t>22-0175</t>
+  </si>
+  <si>
+    <t>22-0176</t>
+  </si>
+  <si>
+    <t>22-0177</t>
+  </si>
+  <si>
+    <t>22-0178</t>
+  </si>
+  <si>
+    <t>22-0179</t>
+  </si>
+  <si>
+    <t>22-0180</t>
+  </si>
+  <si>
+    <t>14.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0181</t>
+  </si>
+  <si>
+    <t>16.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0182</t>
+  </si>
+  <si>
+    <t>20.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0183</t>
+  </si>
+  <si>
+    <t>26.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0184</t>
+  </si>
+  <si>
+    <t>Contessa</t>
+  </si>
+  <si>
+    <t>28.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0185</t>
+  </si>
+  <si>
+    <t>29.09.2022.</t>
+  </si>
+  <si>
+    <t>22-0186</t>
+  </si>
+  <si>
+    <t>05.10.2022.</t>
+  </si>
+  <si>
+    <t>22-0187</t>
+  </si>
+  <si>
+    <t>22-0188</t>
+  </si>
+  <si>
+    <t>Med Kompas</t>
+  </si>
+  <si>
+    <t>22-0189</t>
+  </si>
+  <si>
+    <t>22-0190</t>
+  </si>
+  <si>
+    <t>22-0191</t>
+  </si>
+  <si>
+    <t>22-0192</t>
+  </si>
+  <si>
+    <t>22-0193</t>
+  </si>
+  <si>
+    <t>22-0194</t>
+  </si>
+  <si>
+    <t>22-0195</t>
+  </si>
+  <si>
+    <t>22-0196</t>
+  </si>
+  <si>
+    <t>22-0197</t>
+  </si>
+  <si>
+    <t>22-0198</t>
+  </si>
+  <si>
+    <t>22-0199</t>
+  </si>
+  <si>
+    <t>22-0200</t>
+  </si>
+  <si>
+    <t>22-0201</t>
+  </si>
+  <si>
+    <t>23.08.2022.</t>
   </si>
 </sst>
 </file>
@@ -2006,7 +2189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2048,12 +2231,57 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2236,47 +2464,6 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -2397,18 +2584,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{61B352A4-D6A6-46E6-A50B-9A1CD5208070}" name="Table15" displayName="Table15" ref="A1:F423" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F423" xr:uid="{7AADC68E-98BA-45A9-88EB-FA8E47C21085}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{61B352A4-D6A6-46E6-A50B-9A1CD5208070}" name="Table15" displayName="Table15" ref="A1:F468" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F468" xr:uid="{7AADC68E-98BA-45A9-88EB-FA8E47C21085}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F423">
     <sortCondition ref="B1:B423"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DA99C80C-EA37-42EB-A25C-335AC672DF10}" name="Br." dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8A0EED7A-F881-4866-832B-48B671DBB3CC}" name="Datum" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{63DE4C06-8811-403E-9B56-B10E70F0D042}" name="Broj fakture" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6EBA4B34-0F27-4583-BEAC-3F86D280865F}" name="Kupac" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{C507D0FA-8214-4F32-AD75-445B68CCB309}" name="Usluga" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{BDFB6C30-F148-43F2-A974-CA26E6008DFE}" name="Iznos fakture" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8A0EED7A-F881-4866-832B-48B671DBB3CC}" name="Datum" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{63DE4C06-8811-403E-9B56-B10E70F0D042}" name="Broj fakture" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{6EBA4B34-0F27-4583-BEAC-3F86D280865F}" name="Kupac" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{C507D0FA-8214-4F32-AD75-445B68CCB309}" name="Usluga" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BDFB6C30-F148-43F2-A974-CA26E6008DFE}" name="Iznos fakture" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2711,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E7FC71-59A6-4427-96D9-769599653D8F}">
-  <dimension ref="A1:F423"/>
+  <dimension ref="A1:P469"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
+      <selection activeCell="D474" sqref="D474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,6 +2912,8 @@
     <col min="4" max="4" width="49.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -11047,7 +11236,7 @@
         <v>157510</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A417" s="5">
         <v>416</v>
       </c>
@@ -11067,7 +11256,7 @@
         <v>24650</v>
       </c>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A418" s="5">
         <v>417</v>
       </c>
@@ -11087,7 +11276,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A419" s="5">
         <v>418</v>
       </c>
@@ -11107,7 +11296,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A420" s="5">
         <v>419</v>
       </c>
@@ -11127,7 +11316,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A421" s="5">
         <v>420</v>
       </c>
@@ -11147,7 +11336,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A422" s="5">
         <v>421</v>
       </c>
@@ -11167,7 +11356,7 @@
         <v>70600</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A423" s="5">
         <v>422</v>
       </c>
@@ -11185,6 +11374,1874 @@
       </c>
       <c r="F423" s="9">
         <v>200000</v>
+      </c>
+    </row>
+    <row r="424" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A424" s="5">
+        <v>423</v>
+      </c>
+      <c r="B424" s="12">
+        <v>44796</v>
+      </c>
+      <c r="C424" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="D424" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E424" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F424" s="9">
+        <v>7800</v>
+      </c>
+      <c r="I424" t="s">
+        <v>660</v>
+      </c>
+      <c r="K424">
+        <v>2022</v>
+      </c>
+      <c r="L424" t="str">
+        <f>RIGHT(LEFT(I424,5),2)</f>
+        <v>08</v>
+      </c>
+      <c r="M424" t="str">
+        <f>LEFT(I424,2)</f>
+        <v>23</v>
+      </c>
+      <c r="O424" s="16">
+        <f>DATE(K424,L424,M424)</f>
+        <v>44796</v>
+      </c>
+      <c r="P424">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="425" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A425" s="5">
+        <v>424</v>
+      </c>
+      <c r="B425" s="15">
+        <v>44803</v>
+      </c>
+      <c r="C425" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="D425" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E425" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F425" s="9">
+        <v>6000</v>
+      </c>
+      <c r="I425" t="s">
+        <v>600</v>
+      </c>
+      <c r="K425">
+        <v>2022</v>
+      </c>
+      <c r="L425" t="str">
+        <f t="shared" ref="L425:L469" si="0">RIGHT(LEFT(I425,5),2)</f>
+        <v>08</v>
+      </c>
+      <c r="M425" t="str">
+        <f t="shared" ref="M425:M469" si="1">LEFT(I425,2)</f>
+        <v>30</v>
+      </c>
+      <c r="O425" s="16">
+        <f t="shared" ref="O425:O469" si="2">DATE(K425,L425,M425)</f>
+        <v>44803</v>
+      </c>
+      <c r="P425">
+        <v>44803</v>
+      </c>
+    </row>
+    <row r="426" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A426" s="5">
+        <v>425</v>
+      </c>
+      <c r="B426" s="15">
+        <v>44803</v>
+      </c>
+      <c r="C426" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="D426" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E426" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F426" s="9">
+        <v>25000</v>
+      </c>
+      <c r="I426" t="s">
+        <v>600</v>
+      </c>
+      <c r="K426">
+        <v>2022</v>
+      </c>
+      <c r="L426" t="str">
+        <f t="shared" si="0"/>
+        <v>08</v>
+      </c>
+      <c r="M426" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O426" s="16">
+        <f t="shared" si="2"/>
+        <v>44803</v>
+      </c>
+      <c r="P426">
+        <v>44803</v>
+      </c>
+    </row>
+    <row r="427" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A427" s="5">
+        <v>426</v>
+      </c>
+      <c r="B427" s="15">
+        <v>44803</v>
+      </c>
+      <c r="C427" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="D427" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E427" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F427" s="9">
+        <v>3000</v>
+      </c>
+      <c r="I427" t="s">
+        <v>600</v>
+      </c>
+      <c r="K427">
+        <v>2022</v>
+      </c>
+      <c r="L427" t="str">
+        <f t="shared" si="0"/>
+        <v>08</v>
+      </c>
+      <c r="M427" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O427" s="16">
+        <f t="shared" si="2"/>
+        <v>44803</v>
+      </c>
+      <c r="P427">
+        <v>44803</v>
+      </c>
+    </row>
+    <row r="428" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A428" s="5">
+        <v>427</v>
+      </c>
+      <c r="B428" s="15">
+        <v>44803</v>
+      </c>
+      <c r="C428" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="D428" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E428" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F428" s="9">
+        <v>70000</v>
+      </c>
+      <c r="I428" t="s">
+        <v>600</v>
+      </c>
+      <c r="K428">
+        <v>2022</v>
+      </c>
+      <c r="L428" t="str">
+        <f t="shared" si="0"/>
+        <v>08</v>
+      </c>
+      <c r="M428" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O428" s="16">
+        <f t="shared" si="2"/>
+        <v>44803</v>
+      </c>
+      <c r="P428">
+        <v>44803</v>
+      </c>
+    </row>
+    <row r="429" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A429" s="5">
+        <v>428</v>
+      </c>
+      <c r="B429" s="15">
+        <v>44803</v>
+      </c>
+      <c r="C429" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="D429" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E429" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F429" s="9">
+        <v>7000</v>
+      </c>
+      <c r="I429" t="s">
+        <v>600</v>
+      </c>
+      <c r="K429">
+        <v>2022</v>
+      </c>
+      <c r="L429" t="str">
+        <f t="shared" si="0"/>
+        <v>08</v>
+      </c>
+      <c r="M429" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="O429" s="16">
+        <f t="shared" si="2"/>
+        <v>44803</v>
+      </c>
+      <c r="P429">
+        <v>44803</v>
+      </c>
+    </row>
+    <row r="430" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A430" s="5">
+        <v>429</v>
+      </c>
+      <c r="B430" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C430" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="D430" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E430" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F430" s="9">
+        <v>9000</v>
+      </c>
+      <c r="I430" t="s">
+        <v>606</v>
+      </c>
+      <c r="K430">
+        <v>2022</v>
+      </c>
+      <c r="L430" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M430" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O430" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P430">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="431" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A431" s="5">
+        <v>430</v>
+      </c>
+      <c r="B431" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C431" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="D431" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E431" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F431" s="9">
+        <v>10000</v>
+      </c>
+      <c r="I431" t="s">
+        <v>606</v>
+      </c>
+      <c r="K431">
+        <v>2022</v>
+      </c>
+      <c r="L431" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M431" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O431" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P431">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="432" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A432" s="5">
+        <v>431</v>
+      </c>
+      <c r="B432" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C432" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="D432" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E432" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F432" s="9">
+        <v>6000</v>
+      </c>
+      <c r="I432" t="s">
+        <v>606</v>
+      </c>
+      <c r="K432">
+        <v>2022</v>
+      </c>
+      <c r="L432" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M432" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O432" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P432">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="433" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A433" s="5">
+        <v>432</v>
+      </c>
+      <c r="B433" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C433" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="D433" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E433" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F433" s="9">
+        <v>7000</v>
+      </c>
+      <c r="I433" t="s">
+        <v>606</v>
+      </c>
+      <c r="K433">
+        <v>2022</v>
+      </c>
+      <c r="L433" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M433" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O433" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P433">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="434" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A434" s="5">
+        <v>433</v>
+      </c>
+      <c r="B434" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C434" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="D434" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E434" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F434" s="9">
+        <v>7000</v>
+      </c>
+      <c r="I434" t="s">
+        <v>606</v>
+      </c>
+      <c r="K434">
+        <v>2022</v>
+      </c>
+      <c r="L434" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M434" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O434" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P434">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="435" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A435" s="5">
+        <v>434</v>
+      </c>
+      <c r="B435" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C435" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="D435" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E435" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F435" s="9">
+        <v>8000</v>
+      </c>
+      <c r="I435" t="s">
+        <v>606</v>
+      </c>
+      <c r="K435">
+        <v>2022</v>
+      </c>
+      <c r="L435" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M435" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O435" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P435">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="436" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A436" s="5">
+        <v>435</v>
+      </c>
+      <c r="B436" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C436" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="D436" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="E436" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F436" s="9">
+        <v>4200</v>
+      </c>
+      <c r="I436" t="s">
+        <v>606</v>
+      </c>
+      <c r="K436">
+        <v>2022</v>
+      </c>
+      <c r="L436" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M436" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O436" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P436">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="437" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A437" s="5">
+        <v>436</v>
+      </c>
+      <c r="B437" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C437" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="D437" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="E437" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F437" s="9">
+        <v>4200</v>
+      </c>
+      <c r="I437" t="s">
+        <v>606</v>
+      </c>
+      <c r="K437">
+        <v>2022</v>
+      </c>
+      <c r="L437" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M437" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O437" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P437">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="438" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A438" s="5">
+        <v>437</v>
+      </c>
+      <c r="B438" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C438" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="D438" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E438" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F438" s="9">
+        <v>218620</v>
+      </c>
+      <c r="I438" t="s">
+        <v>606</v>
+      </c>
+      <c r="K438">
+        <v>2022</v>
+      </c>
+      <c r="L438" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M438" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O438" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P438">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="439" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A439" s="5">
+        <v>438</v>
+      </c>
+      <c r="B439" s="15">
+        <v>44805</v>
+      </c>
+      <c r="C439" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="D439" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="E439" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F439" s="9">
+        <v>30000</v>
+      </c>
+      <c r="I439" t="s">
+        <v>606</v>
+      </c>
+      <c r="K439">
+        <v>2022</v>
+      </c>
+      <c r="L439" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M439" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="O439" s="16">
+        <f t="shared" si="2"/>
+        <v>44805</v>
+      </c>
+      <c r="P439">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="440" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A440" s="5">
+        <v>439</v>
+      </c>
+      <c r="B440" s="15">
+        <v>44810</v>
+      </c>
+      <c r="C440" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="D440" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E440" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F440" s="9">
+        <v>9000</v>
+      </c>
+      <c r="I440" t="s">
+        <v>618</v>
+      </c>
+      <c r="K440">
+        <v>2022</v>
+      </c>
+      <c r="L440" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M440" t="str">
+        <f t="shared" si="1"/>
+        <v>06</v>
+      </c>
+      <c r="O440" s="16">
+        <f t="shared" si="2"/>
+        <v>44810</v>
+      </c>
+      <c r="P440">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="441" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A441" s="5">
+        <v>440</v>
+      </c>
+      <c r="B441" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C441" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="D441" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E441" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F441" s="9">
+        <v>6000</v>
+      </c>
+      <c r="I441" t="s">
+        <v>621</v>
+      </c>
+      <c r="K441">
+        <v>2022</v>
+      </c>
+      <c r="L441" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M441" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O441" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P441">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="442" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A442" s="5">
+        <v>441</v>
+      </c>
+      <c r="B442" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C442" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="D442" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E442" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F442" s="9">
+        <v>10500</v>
+      </c>
+      <c r="I442" t="s">
+        <v>621</v>
+      </c>
+      <c r="K442">
+        <v>2022</v>
+      </c>
+      <c r="L442" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M442" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O442" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P442">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="443" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A443" s="5">
+        <v>442</v>
+      </c>
+      <c r="B443" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C443" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="D443" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E443" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F443" s="9">
+        <v>4400</v>
+      </c>
+      <c r="I443" t="s">
+        <v>621</v>
+      </c>
+      <c r="K443">
+        <v>2022</v>
+      </c>
+      <c r="L443" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M443" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O443" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P443">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="444" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A444" s="5">
+        <v>443</v>
+      </c>
+      <c r="B444" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C444" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="D444" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="E444" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F444" s="9">
+        <v>4400</v>
+      </c>
+      <c r="I444" t="s">
+        <v>621</v>
+      </c>
+      <c r="K444">
+        <v>2022</v>
+      </c>
+      <c r="L444" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M444" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O444" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P444">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="445" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A445" s="5">
+        <v>444</v>
+      </c>
+      <c r="B445" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C445" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="D445" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="E445" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F445" s="9">
+        <v>4400</v>
+      </c>
+      <c r="I445" t="s">
+        <v>621</v>
+      </c>
+      <c r="K445">
+        <v>2022</v>
+      </c>
+      <c r="L445" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M445" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O445" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P445">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="446" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A446" s="5">
+        <v>445</v>
+      </c>
+      <c r="B446" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C446" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="D446" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="E446" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F446" s="9">
+        <v>4400</v>
+      </c>
+      <c r="I446" t="s">
+        <v>621</v>
+      </c>
+      <c r="K446">
+        <v>2022</v>
+      </c>
+      <c r="L446" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M446" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O446" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P446">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A447" s="5">
+        <v>446</v>
+      </c>
+      <c r="B447" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C447" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="D447" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="E447" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F447" s="9">
+        <v>4400</v>
+      </c>
+      <c r="I447" t="s">
+        <v>621</v>
+      </c>
+      <c r="K447">
+        <v>2022</v>
+      </c>
+      <c r="L447" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M447" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O447" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P447">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A448" s="5">
+        <v>447</v>
+      </c>
+      <c r="B448" s="15">
+        <v>44816</v>
+      </c>
+      <c r="C448" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="D448" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E448" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F448" s="9">
+        <v>23460</v>
+      </c>
+      <c r="I448" t="s">
+        <v>621</v>
+      </c>
+      <c r="K448">
+        <v>2022</v>
+      </c>
+      <c r="L448" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M448" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O448" s="16">
+        <f t="shared" si="2"/>
+        <v>44816</v>
+      </c>
+      <c r="P448">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A449" s="5">
+        <v>448</v>
+      </c>
+      <c r="B449" s="15">
+        <v>44818</v>
+      </c>
+      <c r="C449" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="D449" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E449" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F449" s="9">
+        <v>100000</v>
+      </c>
+      <c r="I449" t="s">
+        <v>630</v>
+      </c>
+      <c r="K449">
+        <v>2022</v>
+      </c>
+      <c r="L449" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M449" t="str">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="O449" s="16">
+        <f t="shared" si="2"/>
+        <v>44818</v>
+      </c>
+      <c r="P449">
+        <v>44818</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A450" s="5">
+        <v>449</v>
+      </c>
+      <c r="B450" s="15">
+        <v>44820</v>
+      </c>
+      <c r="C450" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="D450" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E450" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F450" s="9">
+        <v>7050</v>
+      </c>
+      <c r="I450" t="s">
+        <v>632</v>
+      </c>
+      <c r="K450">
+        <v>2022</v>
+      </c>
+      <c r="L450" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M450" t="str">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="O450" s="16">
+        <f t="shared" si="2"/>
+        <v>44820</v>
+      </c>
+      <c r="P450">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A451" s="5">
+        <v>450</v>
+      </c>
+      <c r="B451" s="15">
+        <v>44824</v>
+      </c>
+      <c r="C451" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="D451" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="E451" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F451" s="9">
+        <v>481000</v>
+      </c>
+      <c r="I451" t="s">
+        <v>634</v>
+      </c>
+      <c r="K451">
+        <v>2022</v>
+      </c>
+      <c r="L451" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M451" t="str">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="O451" s="16">
+        <f t="shared" si="2"/>
+        <v>44824</v>
+      </c>
+      <c r="P451">
+        <v>44824</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A452" s="5">
+        <v>451</v>
+      </c>
+      <c r="B452" s="15">
+        <v>44830</v>
+      </c>
+      <c r="C452" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="D452" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E452" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F452" s="9">
+        <v>2820</v>
+      </c>
+      <c r="I452" t="s">
+        <v>636</v>
+      </c>
+      <c r="K452">
+        <v>2022</v>
+      </c>
+      <c r="L452" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M452" t="str">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="O452" s="16">
+        <f t="shared" si="2"/>
+        <v>44830</v>
+      </c>
+      <c r="P452">
+        <v>44830</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A453" s="5">
+        <v>452</v>
+      </c>
+      <c r="B453" s="15">
+        <v>44832</v>
+      </c>
+      <c r="C453" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="D453" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E453" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F453" s="9">
+        <v>120000</v>
+      </c>
+      <c r="I453" t="s">
+        <v>639</v>
+      </c>
+      <c r="K453">
+        <v>2022</v>
+      </c>
+      <c r="L453" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M453" t="str">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="O453" s="16">
+        <f t="shared" si="2"/>
+        <v>44832</v>
+      </c>
+      <c r="P453">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A454" s="5">
+        <v>453</v>
+      </c>
+      <c r="B454" s="15">
+        <v>44833</v>
+      </c>
+      <c r="C454" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="D454" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E454" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F454" s="9">
+        <v>30000</v>
+      </c>
+      <c r="I454" t="s">
+        <v>641</v>
+      </c>
+      <c r="K454">
+        <v>2022</v>
+      </c>
+      <c r="L454" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
+      </c>
+      <c r="M454" t="str">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="O454" s="16">
+        <f t="shared" si="2"/>
+        <v>44833</v>
+      </c>
+      <c r="P454">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A455" s="5">
+        <v>454</v>
+      </c>
+      <c r="B455" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C455" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="D455" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="E455" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F455" s="9">
+        <v>3500</v>
+      </c>
+      <c r="I455" t="s">
+        <v>643</v>
+      </c>
+      <c r="K455">
+        <v>2022</v>
+      </c>
+      <c r="L455" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M455" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O455" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P455">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="456" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A456" s="5">
+        <v>455</v>
+      </c>
+      <c r="B456" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C456" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="D456" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E456" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F456" s="9">
+        <v>3000</v>
+      </c>
+      <c r="I456" t="s">
+        <v>643</v>
+      </c>
+      <c r="K456">
+        <v>2022</v>
+      </c>
+      <c r="L456" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M456" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O456" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P456">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A457" s="5">
+        <v>456</v>
+      </c>
+      <c r="B457" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C457" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="D457" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E457" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F457" s="9">
+        <v>7800</v>
+      </c>
+      <c r="I457" t="s">
+        <v>643</v>
+      </c>
+      <c r="K457">
+        <v>2022</v>
+      </c>
+      <c r="L457" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M457" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O457" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P457">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="458" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A458" s="5">
+        <v>457</v>
+      </c>
+      <c r="B458" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C458" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="D458" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E458" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F458" s="9">
+        <v>6000</v>
+      </c>
+      <c r="I458" t="s">
+        <v>643</v>
+      </c>
+      <c r="K458">
+        <v>2022</v>
+      </c>
+      <c r="L458" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M458" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O458" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P458">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A459" s="5">
+        <v>458</v>
+      </c>
+      <c r="B459" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C459" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="D459" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="E459" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F459" s="9">
+        <v>10000</v>
+      </c>
+      <c r="I459" t="s">
+        <v>643</v>
+      </c>
+      <c r="K459">
+        <v>2022</v>
+      </c>
+      <c r="L459" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M459" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O459" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P459">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A460" s="5">
+        <v>459</v>
+      </c>
+      <c r="B460" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C460" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="D460" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E460" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F460" s="9">
+        <v>4000</v>
+      </c>
+      <c r="I460" t="s">
+        <v>643</v>
+      </c>
+      <c r="K460">
+        <v>2022</v>
+      </c>
+      <c r="L460" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M460" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O460" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P460">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A461" s="5">
+        <v>460</v>
+      </c>
+      <c r="B461" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C461" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="D461" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E461" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F461" s="9">
+        <v>11000</v>
+      </c>
+      <c r="I461" t="s">
+        <v>643</v>
+      </c>
+      <c r="K461">
+        <v>2022</v>
+      </c>
+      <c r="L461" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M461" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O461" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P461">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="462" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A462" s="5">
+        <v>461</v>
+      </c>
+      <c r="B462" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C462" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="D462" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E462" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F462" s="9">
+        <v>9000</v>
+      </c>
+      <c r="I462" t="s">
+        <v>643</v>
+      </c>
+      <c r="K462">
+        <v>2022</v>
+      </c>
+      <c r="L462" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M462" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O462" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P462">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A463" s="5">
+        <v>462</v>
+      </c>
+      <c r="B463" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C463" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="D463" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E463" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F463" s="9">
+        <v>10000</v>
+      </c>
+      <c r="I463" t="s">
+        <v>643</v>
+      </c>
+      <c r="K463">
+        <v>2022</v>
+      </c>
+      <c r="L463" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M463" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O463" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P463">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A464" s="5">
+        <v>463</v>
+      </c>
+      <c r="B464" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C464" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="D464" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E464" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F464" s="9">
+        <v>6000</v>
+      </c>
+      <c r="I464" t="s">
+        <v>643</v>
+      </c>
+      <c r="K464">
+        <v>2022</v>
+      </c>
+      <c r="L464" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M464" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O464" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P464">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="465" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A465" s="5">
+        <v>464</v>
+      </c>
+      <c r="B465" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C465" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="D465" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E465" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F465" s="9">
+        <v>7000</v>
+      </c>
+      <c r="I465" t="s">
+        <v>643</v>
+      </c>
+      <c r="K465">
+        <v>2022</v>
+      </c>
+      <c r="L465" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M465" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O465" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P465">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="466" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A466" s="5">
+        <v>465</v>
+      </c>
+      <c r="B466" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C466" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="D466" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E466" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F466" s="9">
+        <v>7000</v>
+      </c>
+      <c r="I466" t="s">
+        <v>643</v>
+      </c>
+      <c r="K466">
+        <v>2022</v>
+      </c>
+      <c r="L466" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M466" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O466" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P466">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="467" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A467" s="5">
+        <v>466</v>
+      </c>
+      <c r="B467" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C467" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="D467" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E467" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F467" s="9">
+        <v>8000</v>
+      </c>
+      <c r="I467" t="s">
+        <v>643</v>
+      </c>
+      <c r="K467">
+        <v>2022</v>
+      </c>
+      <c r="L467" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M467" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O467" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P467">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="468" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A468" s="5">
+        <v>467</v>
+      </c>
+      <c r="B468" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C468" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="D468" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E468" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F468" s="9">
+        <v>6980</v>
+      </c>
+      <c r="I468" t="s">
+        <v>643</v>
+      </c>
+      <c r="K468">
+        <v>2022</v>
+      </c>
+      <c r="L468" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M468" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O468" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P468">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="469" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I469" t="s">
+        <v>643</v>
+      </c>
+      <c r="K469">
+        <v>2022</v>
+      </c>
+      <c r="L469" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M469" t="str">
+        <f t="shared" si="1"/>
+        <v>05</v>
+      </c>
+      <c r="O469" s="16">
+        <f t="shared" si="2"/>
+        <v>44839</v>
+      </c>
+      <c r="P469">
+        <v>44839</v>
       </c>
     </row>
   </sheetData>
@@ -11200,7 +13257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB691B2-6918-4482-A2EB-53046D0DB009}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ver 0.022 prevedeno na srpski
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mihas\Programming\Python\Projects\KPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05EEBF-6E83-43B0-807E-68235DD8F1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B5A65B-6120-4F31-87CB-95A90ADBDF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EDA8619-E0A5-4851-A543-B76F1F64E136}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5EDA8619-E0A5-4851-A543-B76F1F64E136}"/>
   </bookViews>
   <sheets>
-    <sheet name="pripremljen 2021 2022" sheetId="4" r:id="rId1"/>
+    <sheet name="pripremljen 2021 2022 backup" sheetId="4" r:id="rId1"/>
     <sheet name="Users" sheetId="5" r:id="rId2"/>
     <sheet name="Companys" sheetId="6" r:id="rId3"/>
+    <sheet name="pripremljen 2021 2022" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'pripremljen 2021 2022'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'pripremljen 2021 2022'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'pripremljen 2021 2022 backup'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="661">
   <si>
     <t>Br.</t>
   </si>
@@ -2240,7 +2242,171 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2274,6 +2440,130 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -2464,6 +2754,47 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -2584,18 +2915,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{61B352A4-D6A6-46E6-A50B-9A1CD5208070}" name="Table15" displayName="Table15" ref="A1:F468" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{61B352A4-D6A6-46E6-A50B-9A1CD5208070}" name="Table15" displayName="Table15" ref="A1:F468" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:F468" xr:uid="{7AADC68E-98BA-45A9-88EB-FA8E47C21085}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F423">
     <sortCondition ref="B1:B423"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DA99C80C-EA37-42EB-A25C-335AC672DF10}" name="Br." dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8A0EED7A-F881-4866-832B-48B671DBB3CC}" name="Datum" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{63DE4C06-8811-403E-9B56-B10E70F0D042}" name="Broj fakture" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{6EBA4B34-0F27-4583-BEAC-3F86D280865F}" name="Kupac" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{C507D0FA-8214-4F32-AD75-445B68CCB309}" name="Usluga" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BDFB6C30-F148-43F2-A974-CA26E6008DFE}" name="Iznos fakture" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{DA99C80C-EA37-42EB-A25C-335AC672DF10}" name="Br." dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{8A0EED7A-F881-4866-832B-48B671DBB3CC}" name="Datum" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{63DE4C06-8811-403E-9B56-B10E70F0D042}" name="Broj fakture" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{6EBA4B34-0F27-4583-BEAC-3F86D280865F}" name="Kupac" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{C507D0FA-8214-4F32-AD75-445B68CCB309}" name="Usluga" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{BDFB6C30-F148-43F2-A974-CA26E6008DFE}" name="Iznos fakture" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D1C4101C-4961-49FC-97F5-C489694C03E5}" name="Table152" displayName="Table152" ref="A1:F13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F13" xr:uid="{7AADC68E-98BA-45A9-88EB-FA8E47C21085}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{30BB2D7D-318A-482E-B548-7016BCB106D2}" name="Br." dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3649A5BC-F2B5-45E8-91DF-5601EC9734F2}" name="Datum" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{0E65D0A5-B428-4930-BA36-8B4D3A9C7DE8}" name="Broj fakture" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D8CC37A0-A0A8-40C1-8B4F-9B278B2944B6}" name="Kupac" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{FA792121-F52B-4BA4-988D-D8375919681B}" name="Usluga" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2CEB41D1-88FC-41DE-BD5A-693F1276C309}" name="Iznos fakture" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2900,8 +3246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E7FC71-59A6-4427-96D9-769599653D8F}">
   <dimension ref="A1:P469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
-      <selection activeCell="D474" sqref="D474"/>
+    <sheetView topLeftCell="A437" workbookViewId="0">
+      <selection activeCell="E449" sqref="E449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13612,4 +13958,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A14018-4B58-4503-8C90-813409BFB0B8}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>456</v>
+      </c>
+      <c r="B2" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>457</v>
+      </c>
+      <c r="B3" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>458</v>
+      </c>
+      <c r="B4" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>459</v>
+      </c>
+      <c r="B5" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>460</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>461</v>
+      </c>
+      <c r="B7" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>462</v>
+      </c>
+      <c r="B8" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>463</v>
+      </c>
+      <c r="B9" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="9">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>464</v>
+      </c>
+      <c r="B10" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>465</v>
+      </c>
+      <c r="B11" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>466</v>
+      </c>
+      <c r="B12" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="9">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>467</v>
+      </c>
+      <c r="B13" s="15">
+        <v>44839</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F13" s="9">
+        <v>6980</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>